<commit_message>
Ajout du formulaire de contact
</commit_message>
<xml_diff>
--- a/doc/scénarii_CU.xlsx
+++ b/doc/scénarii_CU.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="36" windowWidth="17064" windowHeight="7176" tabRatio="806" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="576" yWindow="36" windowWidth="17064" windowHeight="7176" tabRatio="806"/>
   </bookViews>
   <sheets>
     <sheet name="CU1 devenir membre" sheetId="1" r:id="rId1"/>
@@ -191,9 +191,6 @@
     <t>10. L'administrateur vérifie les informations du nouveau membre</t>
   </si>
   <si>
-    <t>11. L'administrateur valide les informations saisie du nouvel internaute</t>
-  </si>
-  <si>
     <t>12. Le nouveau membre est informé qui fait partie de l'association.</t>
   </si>
   <si>
@@ -751,6 +748,9 @@
   </si>
   <si>
     <t>4. L'internaute non membre ou le membre de l'association saisit ses coordonnées bancaires</t>
+  </si>
+  <si>
+    <t>11. L'administrateur valide les informations saisies du nouvel internaute</t>
   </si>
 </sst>
 </file>
@@ -1133,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1217,7 +1217,7 @@
     <row r="16" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1267,12 +1267,12 @@
     </row>
     <row r="26" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>38</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1323,17 +1323,17 @@
     </row>
     <row r="38" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1377,7 +1377,7 @@
     <row r="50" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1399,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1414,25 +1414,25 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" s="7"/>
     </row>
@@ -1484,37 +1484,37 @@
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1526,49 +1526,49 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1580,19 +1580,19 @@
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1619,14 +1619,14 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1639,7 +1639,7 @@
   <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B16" sqref="B16:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1653,25 +1653,25 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1704,7 +1704,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" s="1"/>
     </row>
@@ -1717,13 +1717,13 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1735,19 +1735,19 @@
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1765,12 +1765,12 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1782,31 +1782,31 @@
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1818,13 +1818,13 @@
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1836,31 +1836,31 @@
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1887,14 +1887,14 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1908,7 +1908,7 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B16" sqref="B16:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1922,25 +1922,25 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1973,7 +1973,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" s="1"/>
     </row>
@@ -1986,13 +1986,13 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2004,19 +2004,19 @@
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2034,12 +2034,12 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2051,25 +2051,25 @@
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2081,37 +2081,37 @@
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2138,19 +2138,19 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2178,25 +2178,25 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2229,7 +2229,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" s="1"/>
     </row>
@@ -2242,13 +2242,13 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2260,19 +2260,19 @@
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2290,7 +2290,7 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2302,25 +2302,25 @@
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2332,31 +2332,31 @@
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2390,7 +2390,7 @@
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2417,25 +2417,25 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2481,7 +2481,7 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2493,47 +2493,47 @@
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2545,19 +2545,19 @@
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2569,43 +2569,43 @@
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2617,31 +2617,31 @@
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2675,12 +2675,12 @@
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2693,7 +2693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -2708,25 +2708,25 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2772,19 +2772,19 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2796,62 +2796,62 @@
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2863,121 +2863,121 @@
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2989,43 +2989,43 @@
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -3059,7 +3059,7 @@
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rapport, amélioration du formulaire de mise à jour des profils membre
</commit_message>
<xml_diff>
--- a/doc/scénarii_CU.xlsx
+++ b/doc/scénarii_CU.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="36" windowWidth="17064" windowHeight="7176" tabRatio="806" activeTab="5"/>
+    <workbookView xWindow="576" yWindow="36" windowWidth="17064" windowHeight="7176" tabRatio="806" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CU1 devenir membre" sheetId="1" r:id="rId1"/>
@@ -204,20 +204,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Résumé : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ce cas d'utilisation permet aux membres de s'authentier</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Dates de création et mise à jour : </t>
     </r>
     <r>
@@ -502,9 +488,6 @@
     <t>Le membre se souvient plus de ses identifiants de connexion, il demande alors un nouveau mot de passe en renvoyant son email dans un formulaire; Il reçoit son nouveau mot de passe par mail</t>
   </si>
   <si>
-    <t>SE2 : Le site membre saisit des identifiants invalides</t>
-  </si>
-  <si>
     <t>Les identifiants saisies par le membre sont invalides ou ne sont pas connu du site internet</t>
   </si>
   <si>
@@ -754,6 +737,23 @@
   </si>
   <si>
     <t>La page d'inscription à la newsletter ne s'affiche pas</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Résumé : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ce cas d'utilisation permet aux membres de s'authentifier</t>
+    </r>
+  </si>
+  <si>
+    <t>SE2 : Le membre saisit des identifiants invalides</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1194,7 @@
     </row>
     <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1220,7 +1220,7 @@
     <row r="16" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1270,7 +1270,7 @@
     </row>
     <row r="26" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1326,7 +1326,7 @@
     </row>
     <row r="38" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1380,7 +1380,7 @@
     <row r="50" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1402,7 +1402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -1417,25 +1417,25 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1468,7 +1468,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B11" s="7"/>
     </row>
@@ -1487,37 +1487,37 @@
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1529,49 +1529,49 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1583,19 +1583,19 @@
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1622,14 +1622,14 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1641,8 +1641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1662,19 +1662,19 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1707,7 +1707,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B11" s="1"/>
     </row>
@@ -1720,13 +1720,13 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1738,19 +1738,19 @@
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1768,12 +1768,12 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1785,31 +1785,31 @@
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="6" t="s">
-        <v>105</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1821,13 +1821,13 @@
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1839,31 +1839,31 @@
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1890,14 +1890,14 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1925,25 +1925,25 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1976,7 +1976,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B11" s="1"/>
     </row>
@@ -1989,13 +1989,13 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2007,19 +2007,19 @@
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2037,12 +2037,12 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2054,25 +2054,25 @@
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2084,37 +2084,37 @@
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2141,19 +2141,19 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2181,25 +2181,25 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2245,7 +2245,7 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2257,47 +2257,47 @@
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2309,19 +2309,19 @@
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2333,43 +2333,43 @@
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2381,31 +2381,31 @@
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2439,12 +2439,12 @@
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2457,7 +2457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -2472,25 +2472,25 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2523,7 +2523,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B11" s="1"/>
     </row>
@@ -2536,13 +2536,13 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2554,19 +2554,19 @@
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2584,7 +2584,7 @@
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2596,25 +2596,25 @@
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2626,37 +2626,37 @@
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2690,7 +2690,7 @@
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2717,25 +2717,25 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2781,19 +2781,19 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2805,62 +2805,62 @@
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2872,121 +2872,121 @@
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2998,43 +2998,43 @@
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -3068,7 +3068,7 @@
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>